<commit_message>
making datapull more concise
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v2.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/GitHub/Fiscal-Impact-Measure/documentation/COVID-19 Changes/September/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6339456-5532-D14D-B965-DA85899B0AEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9370B846-0E88-FE46-911C-23A560CCD531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18780" activeTab="1" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -2387,13 +2387,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2766,10 +2766,10 @@
   <dimension ref="A1:AI72"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5970,7 +5970,7 @@
         <v>437574.00006843987</v>
       </c>
       <c r="M58" s="145">
-        <f t="shared" si="45"/>
+        <f>M49+M22-M45</f>
         <v>435863.45738357492</v>
       </c>
       <c r="N58" s="145">
@@ -6395,11 +6395,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F6A688-71E8-4308-9AE6-7C668128D989}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="8" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7993,7 +7993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304CD302-ECA7-4CE9-B89D-A357A53FDBE8}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -8837,7 +8837,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:H11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11146,8 +11146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF29D8-3B4C-4287-8349-C362C52DEB32}">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12261,22 +12261,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="233" t="s">
+      <c r="E6" s="231" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="233"/>
-      <c r="G6" s="233"/>
-      <c r="H6" s="233"/>
-      <c r="I6" s="233"/>
-      <c r="J6" s="233"/>
-      <c r="K6" s="233"/>
-      <c r="L6" s="233"/>
-      <c r="M6" s="233"/>
-      <c r="N6" s="233"/>
-      <c r="O6" s="233"/>
-      <c r="P6" s="233"/>
-      <c r="Q6" s="233"/>
-      <c r="R6" s="233"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="231"/>
+      <c r="H6" s="231"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="231"/>
+      <c r="K6" s="231"/>
+      <c r="L6" s="231"/>
+      <c r="M6" s="231"/>
+      <c r="N6" s="231"/>
+      <c r="O6" s="231"/>
+      <c r="P6" s="231"/>
+      <c r="Q6" s="231"/>
+      <c r="R6" s="231"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="230" t="s">
@@ -13012,21 +13012,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="231" t="s">
+      <c r="H27" s="232" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="231"/>
-      <c r="J27" s="231"/>
-      <c r="K27" s="231"/>
-      <c r="L27" s="231"/>
-      <c r="M27" s="231"/>
-      <c r="N27" s="231"/>
-      <c r="O27" s="231"/>
-      <c r="P27" s="231"/>
-      <c r="Q27" s="231"/>
-      <c r="R27" s="231"/>
-      <c r="S27" s="231"/>
-      <c r="T27" s="231"/>
+      <c r="I27" s="232"/>
+      <c r="J27" s="232"/>
+      <c r="K27" s="232"/>
+      <c r="L27" s="232"/>
+      <c r="M27" s="232"/>
+      <c r="N27" s="232"/>
+      <c r="O27" s="232"/>
+      <c r="P27" s="232"/>
+      <c r="Q27" s="232"/>
+      <c r="R27" s="232"/>
+      <c r="S27" s="232"/>
+      <c r="T27" s="232"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -13342,21 +13342,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="232" t="s">
+      <c r="F37" s="233" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="232"/>
-      <c r="H37" s="232"/>
-      <c r="I37" s="232"/>
-      <c r="J37" s="232"/>
-      <c r="K37" s="232"/>
-      <c r="L37" s="232"/>
-      <c r="M37" s="232"/>
-      <c r="N37" s="232"/>
-      <c r="O37" s="232"/>
-      <c r="P37" s="232"/>
-      <c r="Q37" s="232"/>
-      <c r="R37" s="232"/>
+      <c r="G37" s="233"/>
+      <c r="H37" s="233"/>
+      <c r="I37" s="233"/>
+      <c r="J37" s="233"/>
+      <c r="K37" s="233"/>
+      <c r="L37" s="233"/>
+      <c r="M37" s="233"/>
+      <c r="N37" s="233"/>
+      <c r="O37" s="233"/>
+      <c r="P37" s="233"/>
+      <c r="Q37" s="233"/>
+      <c r="R37" s="233"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -13672,21 +13672,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="231" t="s">
+      <c r="F48" s="232" t="s">
         <v>102</v>
       </c>
-      <c r="G48" s="231"/>
-      <c r="H48" s="231"/>
-      <c r="I48" s="231"/>
-      <c r="J48" s="231"/>
-      <c r="K48" s="231"/>
-      <c r="L48" s="231"/>
-      <c r="M48" s="231"/>
-      <c r="N48" s="231"/>
-      <c r="O48" s="231"/>
-      <c r="P48" s="231"/>
-      <c r="Q48" s="231"/>
-      <c r="R48" s="231"/>
+      <c r="G48" s="232"/>
+      <c r="H48" s="232"/>
+      <c r="I48" s="232"/>
+      <c r="J48" s="232"/>
+      <c r="K48" s="232"/>
+      <c r="L48" s="232"/>
+      <c r="M48" s="232"/>
+      <c r="N48" s="232"/>
+      <c r="O48" s="232"/>
+      <c r="P48" s="232"/>
+      <c r="Q48" s="232"/>
+      <c r="R48" s="232"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -13998,12 +13998,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -14012,6 +14006,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17899,18 +17899,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17933,14 +17933,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -17955,4 +17947,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "making datapull more concise"
This reverts commit a379c3d049edf017ca0dafb371baf2357e4a4088.
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v2.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/GitHub/Fiscal-Impact-Measure/documentation/COVID-19 Changes/September/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9370B846-0E88-FE46-911C-23A560CCD531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6339456-5532-D14D-B965-DA85899B0AEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18780" activeTab="1" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -2387,13 +2387,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2766,10 +2766,10 @@
   <dimension ref="A1:AI72"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5970,7 +5970,7 @@
         <v>437574.00006843987</v>
       </c>
       <c r="M58" s="145">
-        <f>M49+M22-M45</f>
+        <f t="shared" si="45"/>
         <v>435863.45738357492</v>
       </c>
       <c r="N58" s="145">
@@ -6395,11 +6395,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F6A688-71E8-4308-9AE6-7C668128D989}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="8" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F68" sqref="F68"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7993,7 +7993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304CD302-ECA7-4CE9-B89D-A357A53FDBE8}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -8837,7 +8837,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F11" sqref="F11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11146,8 +11146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF29D8-3B4C-4287-8349-C362C52DEB32}">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12261,22 +12261,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="231" t="s">
+      <c r="E6" s="233" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="231"/>
-      <c r="G6" s="231"/>
-      <c r="H6" s="231"/>
-      <c r="I6" s="231"/>
-      <c r="J6" s="231"/>
-      <c r="K6" s="231"/>
-      <c r="L6" s="231"/>
-      <c r="M6" s="231"/>
-      <c r="N6" s="231"/>
-      <c r="O6" s="231"/>
-      <c r="P6" s="231"/>
-      <c r="Q6" s="231"/>
-      <c r="R6" s="231"/>
+      <c r="F6" s="233"/>
+      <c r="G6" s="233"/>
+      <c r="H6" s="233"/>
+      <c r="I6" s="233"/>
+      <c r="J6" s="233"/>
+      <c r="K6" s="233"/>
+      <c r="L6" s="233"/>
+      <c r="M6" s="233"/>
+      <c r="N6" s="233"/>
+      <c r="O6" s="233"/>
+      <c r="P6" s="233"/>
+      <c r="Q6" s="233"/>
+      <c r="R6" s="233"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="230" t="s">
@@ -13012,21 +13012,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="232" t="s">
+      <c r="H27" s="231" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="232"/>
-      <c r="J27" s="232"/>
-      <c r="K27" s="232"/>
-      <c r="L27" s="232"/>
-      <c r="M27" s="232"/>
-      <c r="N27" s="232"/>
-      <c r="O27" s="232"/>
-      <c r="P27" s="232"/>
-      <c r="Q27" s="232"/>
-      <c r="R27" s="232"/>
-      <c r="S27" s="232"/>
-      <c r="T27" s="232"/>
+      <c r="I27" s="231"/>
+      <c r="J27" s="231"/>
+      <c r="K27" s="231"/>
+      <c r="L27" s="231"/>
+      <c r="M27" s="231"/>
+      <c r="N27" s="231"/>
+      <c r="O27" s="231"/>
+      <c r="P27" s="231"/>
+      <c r="Q27" s="231"/>
+      <c r="R27" s="231"/>
+      <c r="S27" s="231"/>
+      <c r="T27" s="231"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -13342,21 +13342,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="233" t="s">
+      <c r="F37" s="232" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="233"/>
-      <c r="H37" s="233"/>
-      <c r="I37" s="233"/>
-      <c r="J37" s="233"/>
-      <c r="K37" s="233"/>
-      <c r="L37" s="233"/>
-      <c r="M37" s="233"/>
-      <c r="N37" s="233"/>
-      <c r="O37" s="233"/>
-      <c r="P37" s="233"/>
-      <c r="Q37" s="233"/>
-      <c r="R37" s="233"/>
+      <c r="G37" s="232"/>
+      <c r="H37" s="232"/>
+      <c r="I37" s="232"/>
+      <c r="J37" s="232"/>
+      <c r="K37" s="232"/>
+      <c r="L37" s="232"/>
+      <c r="M37" s="232"/>
+      <c r="N37" s="232"/>
+      <c r="O37" s="232"/>
+      <c r="P37" s="232"/>
+      <c r="Q37" s="232"/>
+      <c r="R37" s="232"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -13672,21 +13672,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="232" t="s">
+      <c r="F48" s="231" t="s">
         <v>102</v>
       </c>
-      <c r="G48" s="232"/>
-      <c r="H48" s="232"/>
-      <c r="I48" s="232"/>
-      <c r="J48" s="232"/>
-      <c r="K48" s="232"/>
-      <c r="L48" s="232"/>
-      <c r="M48" s="232"/>
-      <c r="N48" s="232"/>
-      <c r="O48" s="232"/>
-      <c r="P48" s="232"/>
-      <c r="Q48" s="232"/>
-      <c r="R48" s="232"/>
+      <c r="G48" s="231"/>
+      <c r="H48" s="231"/>
+      <c r="I48" s="231"/>
+      <c r="J48" s="231"/>
+      <c r="K48" s="231"/>
+      <c r="L48" s="231"/>
+      <c r="M48" s="231"/>
+      <c r="N48" s="231"/>
+      <c r="O48" s="231"/>
+      <c r="P48" s="231"/>
+      <c r="Q48" s="231"/>
+      <c r="R48" s="231"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -13998,6 +13998,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -14006,12 +14012,6 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17899,18 +17899,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17933,6 +17933,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -17947,12 +17955,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>